<commit_message>
Weekly orders report with summary
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/catering_orders.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/catering_orders.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="1340" windowWidth="46380" windowHeight="26420"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>[ca.cim][ca.klub]</t>
   </si>
@@ -97,12 +97,81 @@
       <t xml:space="preserve">  ([catering.address])</t>
     </r>
   </si>
+  <si>
+    <t>Hétfő</t>
+  </si>
+  <si>
+    <t>Kedd</t>
+  </si>
+  <si>
+    <t>Szerda</t>
+  </si>
+  <si>
+    <t>Csütörtök</t>
+  </si>
+  <si>
+    <t>Péntek</t>
+  </si>
+  <si>
+    <t>Szombat</t>
+  </si>
+  <si>
+    <t>Vasárnap</t>
+  </si>
+  <si>
+    <t>Összesen</t>
+  </si>
+  <si>
+    <t>[summary.menu;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>Adag:</t>
+  </si>
+  <si>
+    <t>Ár:</t>
+  </si>
+  <si>
+    <t>Fizetendő:</t>
+  </si>
+  <si>
+    <t>[total.amount]</t>
+  </si>
+  <si>
+    <t>[total.unit_price]</t>
+  </si>
+  <si>
+    <t>[total.sum;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.4;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.5;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.6;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.7;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[summary.total;ope=tbs:num]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial CE"/>
@@ -148,6 +217,11 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial CE"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -180,8 +254,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -293,11 +457,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,11 +499,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -378,6 +600,15 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -433,6 +664,15 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -830,7 +1070,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -838,81 +1078,182 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="7" customWidth="1"/>
-    <col min="2" max="8" width="3.140625" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.42578125" style="7"/>
+    <col min="1" max="1" width="7.7109375" style="6" customWidth="1"/>
+    <col min="2" max="8" width="5.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16" width="2.28515625" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="9.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="L4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="M4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="N4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="O4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="P4" s="9" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1">
+      <c r="A6" s="17"/>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1">
+      <c r="A9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>